<commit_message>
added end score page
</commit_message>
<xml_diff>
--- a/Wireframe.xlsx
+++ b/Wireframe.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbster\projects\assignments\quizz-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7FDC667C-20B6-4BEE-9008-DCC5F9949E9C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88714E2-84C2-4AE7-B7F1-CF8A5EDF269D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4EC800EC-E53D-40FA-84EE-9D411BD33E65}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{4EC800EC-E53D-40FA-84EE-9D411BD33E65}"/>
   </bookViews>
   <sheets>
     <sheet name="Start-opening page" sheetId="1" r:id="rId1"/>
     <sheet name="Questions" sheetId="2" r:id="rId2"/>
     <sheet name="Correct-incorrect response" sheetId="9" r:id="rId3"/>
     <sheet name="Image links" sheetId="10" r:id="rId4"/>
+    <sheet name="End score" sheetId="11" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -6071,6 +6072,281 @@
           <a:r>
             <a:rPr lang="en-US" sz="1100"/>
             <a:t>Factoid</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rectangle 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C480257-4ED6-4B40-92A4-C0E72D369B35}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1219200" y="365760"/>
+          <a:ext cx="2438400" cy="527685"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Congratulations! </a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>563880</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rectangle 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5BA073B-EC0C-4397-95D6-31F16E0756C6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="571500" y="3307080"/>
+          <a:ext cx="3649980" cy="617220"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>You've made Bill Nye and Neil Degrasse Tyson proud!</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>327660</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="Rectangle 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B22AD7D-3FC9-4838-899B-EB9E9AEA605E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="937260" y="1021080"/>
+          <a:ext cx="3063240" cy="1684020"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>Final</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t> Score: #/8</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:endParaRPr lang="en-US" sz="1100" baseline="0"/>
+        </a:p>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0"/>
+            <a:t>Try again!</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Rectangle: Rounded Corners 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23A5FA64-B5D4-46D2-AA25-482B11A5259A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1905000" y="2209800"/>
+          <a:ext cx="1120140" cy="335280"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" b="1">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>Start Quiz</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -6379,8 +6655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA5BAA4F-CC85-4FE0-BF6C-E1628F0CFEF0}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6503,7 +6779,7 @@
   <dimension ref="C1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6529,7 +6805,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737AAEA3-DCCD-41F4-9989-6E5593947F55}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A52" sqref="A52"/>
     </sheetView>
   </sheetViews>
@@ -6709,4 +6985,19 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId11"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35BA064-E40C-43F0-9026-910D32A32F73}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
q&a js initial and wireframe update
</commit_message>
<xml_diff>
--- a/Wireframe.xlsx
+++ b/Wireframe.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bobbster\projects\assignments\quizz-app\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F88714E2-84C2-4AE7-B7F1-CF8A5EDF269D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{575B4684-6BFC-41F8-9152-E76DC585DB87}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{4EC800EC-E53D-40FA-84EE-9D411BD33E65}"/>
+    <workbookView xWindow="-6768" yWindow="924" windowWidth="13632" windowHeight="8964" firstSheet="2" activeTab="3" xr2:uid="{4EC800EC-E53D-40FA-84EE-9D411BD33E65}"/>
   </bookViews>
   <sheets>
     <sheet name="Start-opening page" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
   <si>
     <t>Images;</t>
   </si>
@@ -124,16 +124,19 @@
     <t>4. Made up of two elements, hydrogen and oxygen and chemical formula is H2O. It means two hydrogen molecules are bonded with one oxygen molecule. Water has three states, when liquid it is called water, when gas it is called vapor and when solid it is called ice.</t>
   </si>
   <si>
-    <t xml:space="preserve">5. Up to 60% of the human adult body is water. Generally, an adult male needs about 3 liters (3.2 quarts) per day while an adult female needs about 2.2 liters (2.3 quarts) per day. </t>
-  </si>
-  <si>
     <t>6. The Kola Superdeep Borehole was just 9 inches in diameter, but at 40,230 feet (12,262 meters) reigns as the deepest hole. It took almost 20 years to reach that 7.5-mile depth—only half the distance or less to the mantle.</t>
   </si>
   <si>
     <t>7. Organisms that use light for the energy needed to make their own food are called producers. In contrast, consumers are creatures that eat producers to get energy. While plants are the best-known producers, algae, cyanobacteria, and some protists also make sugar via photosynthesis.</t>
   </si>
   <si>
-    <t>8. The ring of fire is located in the Pacific Ocean basin. A number of volcanoes form a ring around the basin which is where the name comes from. This area is home to many earthquakes due to volcanic activity and the movement of tectonic plates. The Pacific Ocean contains more than 75,000 volcanoes.</t>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Approximately 60% to over 72% of the human adult body is water. Generally, an adult male needs about 3 liters (3.2 quarts) per day while an adult female needs about 2.2 liters (2.3 quarts) per day. </t>
+  </si>
+  <si>
+    <t>8. The Pacific ocean is the largest and home to locations like the ring of fire is located in the Pacific Ocean basin. A number of volcanoes form a ring around the basin which is where the name comes from. This area is home to many earthquakes due to volcanic activity and the movement of tectonic plates. The Pacific Ocean contains more than 75,000 volcanoes.</t>
   </si>
 </sst>
 </file>
@@ -2645,52 +2648,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>H2O</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1" fontAlgn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>NaOH</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1" fontAlgn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>HCHHCOO</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:pPr lvl="1" fontAlgn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="lt1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>H3O</a:t>
+            <a:t>5. </a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -6674,7 +6632,7 @@
   <dimension ref="A17:K126"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O14" sqref="O14"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6695,6 +6653,11 @@
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="C34" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="35" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2"/>
@@ -6805,8 +6768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{737AAEA3-DCCD-41F4-9989-6E5593947F55}">
   <dimension ref="A1:A51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A52" sqref="A52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6951,22 +6914,22 @@
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -6991,7 +6954,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B35BA064-E40C-43F0-9026-910D32A32F73}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>

</xml_diff>